<commit_message>
melhorando o grafico agora aceitando qualquer arquivo excel e ajeitando a imagem do home
</commit_message>
<xml_diff>
--- a/dados_empresa.xlsx
+++ b/dados_empresa.xlsx
@@ -469,17 +469,17 @@
         <v>44927</v>
       </c>
       <c r="B2" t="n">
-        <v>629</v>
+        <v>765</v>
       </c>
       <c r="C2" t="n">
-        <v>430</v>
+        <v>305</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Peixes</t>
         </is>
       </c>
     </row>
@@ -488,17 +488,17 @@
         <v>44928</v>
       </c>
       <c r="B3" t="n">
-        <v>717</v>
+        <v>915</v>
       </c>
       <c r="C3" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Perfumaria</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
         <v>44929</v>
       </c>
       <c r="B4" t="n">
-        <v>356</v>
+        <v>122</v>
       </c>
       <c r="C4" t="n">
-        <v>131</v>
+        <v>472</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Sucos</t>
         </is>
       </c>
     </row>
@@ -526,17 +526,17 @@
         <v>44930</v>
       </c>
       <c r="B5" t="n">
-        <v>937</v>
+        <v>749</v>
       </c>
       <c r="C5" t="n">
-        <v>106</v>
+        <v>278</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
     </row>
@@ -545,17 +545,17 @@
         <v>44931</v>
       </c>
       <c r="B6" t="n">
-        <v>611</v>
+        <v>840</v>
       </c>
       <c r="C6" t="n">
-        <v>309</v>
+        <v>104</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Utensílios de Cozinha</t>
         </is>
       </c>
     </row>
@@ -564,17 +564,17 @@
         <v>44932</v>
       </c>
       <c r="B7" t="n">
-        <v>439</v>
+        <v>345</v>
       </c>
       <c r="C7" t="n">
-        <v>225</v>
+        <v>302</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Chás</t>
         </is>
       </c>
     </row>
@@ -583,17 +583,17 @@
         <v>44933</v>
       </c>
       <c r="B8" t="n">
-        <v>137</v>
+        <v>769</v>
       </c>
       <c r="C8" t="n">
-        <v>313</v>
+        <v>65</v>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Jardinagem</t>
         </is>
       </c>
     </row>
@@ -602,17 +602,17 @@
         <v>44934</v>
       </c>
       <c r="B9" t="n">
-        <v>212</v>
+        <v>841</v>
       </c>
       <c r="C9" t="n">
-        <v>417</v>
+        <v>52</v>
       </c>
       <c r="D9" t="n">
         <v>9</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Congelados</t>
         </is>
       </c>
     </row>
@@ -621,17 +621,17 @@
         <v>44935</v>
       </c>
       <c r="B10" t="n">
-        <v>333</v>
+        <v>665</v>
       </c>
       <c r="C10" t="n">
-        <v>402</v>
+        <v>162</v>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Jardinagem</t>
         </is>
       </c>
     </row>
@@ -640,17 +640,17 @@
         <v>44936</v>
       </c>
       <c r="B11" t="n">
-        <v>769</v>
+        <v>788</v>
       </c>
       <c r="C11" t="n">
-        <v>399</v>
+        <v>365</v>
       </c>
       <c r="D11" t="n">
         <v>4</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Laticínios</t>
         </is>
       </c>
     </row>
@@ -659,17 +659,17 @@
         <v>44937</v>
       </c>
       <c r="B12" t="n">
-        <v>286</v>
+        <v>340</v>
       </c>
       <c r="C12" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Cereais</t>
         </is>
       </c>
     </row>
@@ -678,17 +678,17 @@
         <v>44938</v>
       </c>
       <c r="B13" t="n">
-        <v>290</v>
+        <v>408</v>
       </c>
       <c r="C13" t="n">
-        <v>415</v>
+        <v>87</v>
       </c>
       <c r="D13" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Snacks</t>
         </is>
       </c>
     </row>
@@ -697,17 +697,17 @@
         <v>44939</v>
       </c>
       <c r="B14" t="n">
-        <v>718</v>
+        <v>119</v>
       </c>
       <c r="C14" t="n">
-        <v>322</v>
+        <v>210</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Livros</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
         <v>44940</v>
       </c>
       <c r="B15" t="n">
-        <v>893</v>
+        <v>136</v>
       </c>
       <c r="C15" t="n">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="D15" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Alimentos</t>
         </is>
       </c>
     </row>
@@ -735,17 +735,17 @@
         <v>44941</v>
       </c>
       <c r="B16" t="n">
-        <v>701</v>
+        <v>942</v>
       </c>
       <c r="C16" t="n">
-        <v>151</v>
+        <v>374</v>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Decoração</t>
         </is>
       </c>
     </row>
@@ -754,17 +754,17 @@
         <v>44942</v>
       </c>
       <c r="B17" t="n">
-        <v>479</v>
+        <v>396</v>
       </c>
       <c r="C17" t="n">
-        <v>466</v>
+        <v>81</v>
       </c>
       <c r="D17" t="n">
         <v>4</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Condimentos</t>
         </is>
       </c>
     </row>
@@ -773,13 +773,13 @@
         <v>44943</v>
       </c>
       <c r="B18" t="n">
-        <v>753</v>
+        <v>496</v>
       </c>
       <c r="C18" t="n">
-        <v>451</v>
+        <v>403</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -792,17 +792,17 @@
         <v>44944</v>
       </c>
       <c r="B19" t="n">
-        <v>627</v>
+        <v>829</v>
       </c>
       <c r="C19" t="n">
-        <v>493</v>
+        <v>87</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Congelados</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
         <v>44945</v>
       </c>
       <c r="B20" t="n">
-        <v>940</v>
+        <v>694</v>
       </c>
       <c r="C20" t="n">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Doces</t>
         </is>
       </c>
     </row>
@@ -830,17 +830,17 @@
         <v>44946</v>
       </c>
       <c r="B21" t="n">
-        <v>890</v>
+        <v>503</v>
       </c>
       <c r="C21" t="n">
-        <v>59</v>
+        <v>385</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Sucos</t>
         </is>
       </c>
     </row>
@@ -849,17 +849,17 @@
         <v>44947</v>
       </c>
       <c r="B22" t="n">
-        <v>940</v>
+        <v>760</v>
       </c>
       <c r="C22" t="n">
-        <v>112</v>
+        <v>232</v>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Sorvetes</t>
         </is>
       </c>
     </row>
@@ -868,17 +868,17 @@
         <v>44948</v>
       </c>
       <c r="B23" t="n">
-        <v>542</v>
+        <v>192</v>
       </c>
       <c r="C23" t="n">
-        <v>121</v>
+        <v>344</v>
       </c>
       <c r="D23" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Especiarias</t>
         </is>
       </c>
     </row>
@@ -887,17 +887,17 @@
         <v>44949</v>
       </c>
       <c r="B24" t="n">
-        <v>180</v>
+        <v>875</v>
       </c>
       <c r="C24" t="n">
-        <v>443</v>
+        <v>312</v>
       </c>
       <c r="D24" t="n">
         <v>7</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Sucos</t>
         </is>
       </c>
     </row>
@@ -906,17 +906,17 @@
         <v>44950</v>
       </c>
       <c r="B25" t="n">
-        <v>902</v>
+        <v>481</v>
       </c>
       <c r="C25" t="n">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Limpeza</t>
         </is>
       </c>
     </row>
@@ -925,17 +925,17 @@
         <v>44951</v>
       </c>
       <c r="B26" t="n">
-        <v>989</v>
+        <v>365</v>
       </c>
       <c r="C26" t="n">
-        <v>441</v>
+        <v>123</v>
       </c>
       <c r="D26" t="n">
         <v>8</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Móveis</t>
         </is>
       </c>
     </row>
@@ -944,17 +944,17 @@
         <v>44952</v>
       </c>
       <c r="B27" t="n">
-        <v>984</v>
+        <v>656</v>
       </c>
       <c r="C27" t="n">
-        <v>477</v>
+        <v>498</v>
       </c>
       <c r="D27" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Padaria</t>
         </is>
       </c>
     </row>
@@ -963,17 +963,17 @@
         <v>44953</v>
       </c>
       <c r="B28" t="n">
-        <v>325</v>
+        <v>528</v>
       </c>
       <c r="C28" t="n">
-        <v>468</v>
+        <v>495</v>
       </c>
       <c r="D28" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Refrigerantes</t>
         </is>
       </c>
     </row>
@@ -982,17 +982,17 @@
         <v>44954</v>
       </c>
       <c r="B29" t="n">
-        <v>756</v>
+        <v>763</v>
       </c>
       <c r="C29" t="n">
-        <v>429</v>
+        <v>283</v>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Grãos</t>
         </is>
       </c>
     </row>
@@ -1001,17 +1001,17 @@
         <v>44955</v>
       </c>
       <c r="B30" t="n">
-        <v>871</v>
+        <v>558</v>
       </c>
       <c r="C30" t="n">
-        <v>282</v>
+        <v>442</v>
       </c>
       <c r="D30" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Jardinagem Avançada</t>
         </is>
       </c>
     </row>
@@ -1020,17 +1020,17 @@
         <v>44956</v>
       </c>
       <c r="B31" t="n">
-        <v>354</v>
+        <v>565</v>
       </c>
       <c r="C31" t="n">
-        <v>293</v>
+        <v>60</v>
       </c>
       <c r="D31" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
     </row>
@@ -1039,17 +1039,17 @@
         <v>44957</v>
       </c>
       <c r="B32" t="n">
-        <v>492</v>
+        <v>944</v>
       </c>
       <c r="C32" t="n">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="D32" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Especiarias</t>
         </is>
       </c>
     </row>
@@ -1058,17 +1058,17 @@
         <v>44958</v>
       </c>
       <c r="B33" t="n">
-        <v>709</v>
+        <v>565</v>
       </c>
       <c r="C33" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Conservas</t>
         </is>
       </c>
     </row>
@@ -1077,17 +1077,17 @@
         <v>44959</v>
       </c>
       <c r="B34" t="n">
-        <v>545</v>
+        <v>273</v>
       </c>
       <c r="C34" t="n">
-        <v>265</v>
+        <v>427</v>
       </c>
       <c r="D34" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
     </row>
@@ -1096,17 +1096,17 @@
         <v>44960</v>
       </c>
       <c r="B35" t="n">
-        <v>155</v>
+        <v>518</v>
       </c>
       <c r="C35" t="n">
-        <v>189</v>
+        <v>237</v>
       </c>
       <c r="D35" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Frutas</t>
         </is>
       </c>
     </row>
@@ -1115,17 +1115,17 @@
         <v>44961</v>
       </c>
       <c r="B36" t="n">
-        <v>592</v>
+        <v>877</v>
       </c>
       <c r="C36" t="n">
-        <v>368</v>
+        <v>473</v>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Utensílios de Cozinha</t>
         </is>
       </c>
     </row>
@@ -1134,17 +1134,17 @@
         <v>44962</v>
       </c>
       <c r="B37" t="n">
-        <v>303</v>
+        <v>137</v>
       </c>
       <c r="C37" t="n">
-        <v>105</v>
+        <v>266</v>
       </c>
       <c r="D37" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
     </row>
@@ -1153,17 +1153,17 @@
         <v>44963</v>
       </c>
       <c r="B38" t="n">
-        <v>229</v>
+        <v>404</v>
       </c>
       <c r="C38" t="n">
-        <v>225</v>
+        <v>132</v>
       </c>
       <c r="D38" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Decoração</t>
         </is>
       </c>
     </row>
@@ -1172,17 +1172,17 @@
         <v>44964</v>
       </c>
       <c r="B39" t="n">
-        <v>504</v>
+        <v>672</v>
       </c>
       <c r="C39" t="n">
-        <v>128</v>
+        <v>477</v>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Jardinagem</t>
         </is>
       </c>
     </row>
@@ -1191,17 +1191,17 @@
         <v>44965</v>
       </c>
       <c r="B40" t="n">
-        <v>825</v>
+        <v>450</v>
       </c>
       <c r="C40" t="n">
-        <v>120</v>
+        <v>365</v>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
     </row>
@@ -1210,17 +1210,17 @@
         <v>44966</v>
       </c>
       <c r="B41" t="n">
-        <v>695</v>
+        <v>450</v>
       </c>
       <c r="C41" t="n">
-        <v>294</v>
+        <v>207</v>
       </c>
       <c r="D41" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Condimentos</t>
         </is>
       </c>
     </row>
@@ -1229,17 +1229,17 @@
         <v>44967</v>
       </c>
       <c r="B42" t="n">
-        <v>495</v>
+        <v>933</v>
       </c>
       <c r="C42" t="n">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Construção</t>
         </is>
       </c>
     </row>
@@ -1248,17 +1248,17 @@
         <v>44968</v>
       </c>
       <c r="B43" t="n">
-        <v>685</v>
+        <v>885</v>
       </c>
       <c r="C43" t="n">
-        <v>328</v>
+        <v>469</v>
       </c>
       <c r="D43" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Doces</t>
         </is>
       </c>
     </row>
@@ -1267,17 +1267,17 @@
         <v>44969</v>
       </c>
       <c r="B44" t="n">
-        <v>717</v>
+        <v>617</v>
       </c>
       <c r="C44" t="n">
-        <v>339</v>
+        <v>191</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Perfumaria</t>
         </is>
       </c>
     </row>
@@ -1286,17 +1286,17 @@
         <v>44970</v>
       </c>
       <c r="B45" t="n">
-        <v>400</v>
+        <v>612</v>
       </c>
       <c r="C45" t="n">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Bebidas</t>
         </is>
       </c>
     </row>
@@ -1305,17 +1305,17 @@
         <v>44971</v>
       </c>
       <c r="B46" t="n">
-        <v>344</v>
+        <v>313</v>
       </c>
       <c r="C46" t="n">
-        <v>497</v>
+        <v>253</v>
       </c>
       <c r="D46" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Café</t>
         </is>
       </c>
     </row>
@@ -1324,17 +1324,17 @@
         <v>44972</v>
       </c>
       <c r="B47" t="n">
-        <v>210</v>
+        <v>523</v>
       </c>
       <c r="C47" t="n">
-        <v>415</v>
+        <v>97</v>
       </c>
       <c r="D47" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Snacks</t>
         </is>
       </c>
     </row>
@@ -1343,17 +1343,17 @@
         <v>44973</v>
       </c>
       <c r="B48" t="n">
-        <v>976</v>
+        <v>780</v>
       </c>
       <c r="C48" t="n">
-        <v>224</v>
+        <v>170</v>
       </c>
       <c r="D48" t="n">
         <v>5</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Doces</t>
         </is>
       </c>
     </row>
@@ -1362,13 +1362,13 @@
         <v>44974</v>
       </c>
       <c r="B49" t="n">
-        <v>800</v>
+        <v>469</v>
       </c>
       <c r="C49" t="n">
-        <v>170</v>
+        <v>372</v>
       </c>
       <c r="D49" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1381,17 +1381,17 @@
         <v>44975</v>
       </c>
       <c r="B50" t="n">
-        <v>193</v>
+        <v>552</v>
       </c>
       <c r="C50" t="n">
-        <v>373</v>
+        <v>118</v>
       </c>
       <c r="D50" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Águas</t>
         </is>
       </c>
     </row>
@@ -1400,17 +1400,17 @@
         <v>44976</v>
       </c>
       <c r="B51" t="n">
-        <v>255</v>
+        <v>395</v>
       </c>
       <c r="C51" t="n">
-        <v>314</v>
+        <v>234</v>
       </c>
       <c r="D51" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Cama, Mesa e Banho</t>
         </is>
       </c>
     </row>
@@ -1419,17 +1419,17 @@
         <v>44977</v>
       </c>
       <c r="B52" t="n">
-        <v>207</v>
+        <v>990</v>
       </c>
       <c r="C52" t="n">
-        <v>450</v>
+        <v>321</v>
       </c>
       <c r="D52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Pet Shop</t>
         </is>
       </c>
     </row>
@@ -1438,17 +1438,17 @@
         <v>44978</v>
       </c>
       <c r="B53" t="n">
-        <v>141</v>
+        <v>536</v>
       </c>
       <c r="C53" t="n">
-        <v>338</v>
+        <v>78</v>
       </c>
       <c r="D53" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Construção</t>
         </is>
       </c>
     </row>
@@ -1457,17 +1457,17 @@
         <v>44979</v>
       </c>
       <c r="B54" t="n">
-        <v>739</v>
+        <v>285</v>
       </c>
       <c r="C54" t="n">
-        <v>360</v>
+        <v>81</v>
       </c>
       <c r="D54" t="n">
         <v>6</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Bebidas</t>
         </is>
       </c>
     </row>
@@ -1476,17 +1476,17 @@
         <v>44980</v>
       </c>
       <c r="B55" t="n">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C55" t="n">
-        <v>138</v>
+        <v>294</v>
       </c>
       <c r="D55" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Laticínios</t>
         </is>
       </c>
     </row>
@@ -1495,17 +1495,17 @@
         <v>44981</v>
       </c>
       <c r="B56" t="n">
-        <v>256</v>
+        <v>893</v>
       </c>
       <c r="C56" t="n">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="D56" t="n">
         <v>2</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Roupas</t>
         </is>
       </c>
     </row>
@@ -1514,17 +1514,17 @@
         <v>44982</v>
       </c>
       <c r="B57" t="n">
-        <v>614</v>
+        <v>658</v>
       </c>
       <c r="C57" t="n">
-        <v>270</v>
+        <v>131</v>
       </c>
       <c r="D57" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Carnes</t>
         </is>
       </c>
     </row>
@@ -1533,17 +1533,17 @@
         <v>44983</v>
       </c>
       <c r="B58" t="n">
-        <v>445</v>
+        <v>721</v>
       </c>
       <c r="C58" t="n">
-        <v>88</v>
+        <v>224</v>
       </c>
       <c r="D58" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Carnes</t>
         </is>
       </c>
     </row>
@@ -1552,17 +1552,17 @@
         <v>44984</v>
       </c>
       <c r="B59" t="n">
-        <v>729</v>
+        <v>851</v>
       </c>
       <c r="C59" t="n">
-        <v>409</v>
+        <v>151</v>
       </c>
       <c r="D59" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Brinquedos</t>
         </is>
       </c>
     </row>
@@ -1571,17 +1571,17 @@
         <v>44985</v>
       </c>
       <c r="B60" t="n">
-        <v>576</v>
+        <v>165</v>
       </c>
       <c r="C60" t="n">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D60" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
     </row>
@@ -1590,17 +1590,17 @@
         <v>44986</v>
       </c>
       <c r="B61" t="n">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="C61" t="n">
-        <v>441</v>
+        <v>300</v>
       </c>
       <c r="D61" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Farmácia</t>
         </is>
       </c>
     </row>
@@ -1609,17 +1609,17 @@
         <v>44987</v>
       </c>
       <c r="B62" t="n">
-        <v>249</v>
+        <v>924</v>
       </c>
       <c r="C62" t="n">
-        <v>341</v>
+        <v>419</v>
       </c>
       <c r="D62" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Congelados</t>
         </is>
       </c>
     </row>
@@ -1628,17 +1628,17 @@
         <v>44988</v>
       </c>
       <c r="B63" t="n">
-        <v>696</v>
+        <v>629</v>
       </c>
       <c r="C63" t="n">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Perfumaria</t>
         </is>
       </c>
     </row>
@@ -1647,17 +1647,17 @@
         <v>44989</v>
       </c>
       <c r="B64" t="n">
-        <v>817</v>
+        <v>393</v>
       </c>
       <c r="C64" t="n">
-        <v>380</v>
+        <v>273</v>
       </c>
       <c r="D64" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Esportes</t>
         </is>
       </c>
     </row>
@@ -1666,17 +1666,17 @@
         <v>44990</v>
       </c>
       <c r="B65" t="n">
-        <v>215</v>
+        <v>382</v>
       </c>
       <c r="C65" t="n">
-        <v>244</v>
+        <v>89</v>
       </c>
       <c r="D65" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Snacks</t>
         </is>
       </c>
     </row>
@@ -1685,17 +1685,17 @@
         <v>44991</v>
       </c>
       <c r="B66" t="n">
-        <v>185</v>
+        <v>120</v>
       </c>
       <c r="C66" t="n">
-        <v>117</v>
+        <v>411</v>
       </c>
       <c r="D66" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Decoração</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
         <v>44992</v>
       </c>
       <c r="B67" t="n">
-        <v>574</v>
+        <v>343</v>
       </c>
       <c r="C67" t="n">
-        <v>59</v>
+        <v>230</v>
       </c>
       <c r="D67" t="n">
         <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Chás</t>
         </is>
       </c>
     </row>
@@ -1723,17 +1723,17 @@
         <v>44993</v>
       </c>
       <c r="B68" t="n">
-        <v>660</v>
+        <v>843</v>
       </c>
       <c r="C68" t="n">
-        <v>347</v>
+        <v>111</v>
       </c>
       <c r="D68" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Cama, Mesa e Banho</t>
         </is>
       </c>
     </row>
@@ -1742,17 +1742,17 @@
         <v>44994</v>
       </c>
       <c r="B69" t="n">
-        <v>617</v>
+        <v>422</v>
       </c>
       <c r="C69" t="n">
-        <v>414</v>
+        <v>288</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Grãos</t>
         </is>
       </c>
     </row>
@@ -1761,17 +1761,17 @@
         <v>44995</v>
       </c>
       <c r="B70" t="n">
-        <v>836</v>
+        <v>674</v>
       </c>
       <c r="C70" t="n">
-        <v>89</v>
+        <v>287</v>
       </c>
       <c r="D70" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Jardinagem Avançada</t>
         </is>
       </c>
     </row>
@@ -1780,17 +1780,17 @@
         <v>44996</v>
       </c>
       <c r="B71" t="n">
-        <v>903</v>
+        <v>238</v>
       </c>
       <c r="C71" t="n">
-        <v>348</v>
+        <v>266</v>
       </c>
       <c r="D71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Grãos</t>
         </is>
       </c>
     </row>
@@ -1799,17 +1799,17 @@
         <v>44997</v>
       </c>
       <c r="B72" t="n">
-        <v>799</v>
+        <v>251</v>
       </c>
       <c r="C72" t="n">
-        <v>348</v>
+        <v>59</v>
       </c>
       <c r="D72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Sorvetes</t>
         </is>
       </c>
     </row>
@@ -1818,17 +1818,17 @@
         <v>44998</v>
       </c>
       <c r="B73" t="n">
-        <v>405</v>
+        <v>541</v>
       </c>
       <c r="C73" t="n">
-        <v>212</v>
+        <v>433</v>
       </c>
       <c r="D73" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Padaria</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
         <v>44999</v>
       </c>
       <c r="B74" t="n">
-        <v>558</v>
+        <v>282</v>
       </c>
       <c r="C74" t="n">
-        <v>139</v>
+        <v>290</v>
       </c>
       <c r="D74" t="n">
         <v>2</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Esportes</t>
         </is>
       </c>
     </row>
@@ -1856,17 +1856,17 @@
         <v>45000</v>
       </c>
       <c r="B75" t="n">
-        <v>275</v>
+        <v>429</v>
       </c>
       <c r="C75" t="n">
-        <v>380</v>
+        <v>82</v>
       </c>
       <c r="D75" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Limpeza</t>
         </is>
       </c>
     </row>
@@ -1875,17 +1875,17 @@
         <v>45001</v>
       </c>
       <c r="B76" t="n">
-        <v>441</v>
+        <v>107</v>
       </c>
       <c r="C76" t="n">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="D76" t="n">
         <v>4</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Higiene Pessoal</t>
         </is>
       </c>
     </row>
@@ -1894,17 +1894,17 @@
         <v>45002</v>
       </c>
       <c r="B77" t="n">
-        <v>573</v>
+        <v>866</v>
       </c>
       <c r="C77" t="n">
-        <v>71</v>
+        <v>450</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Sucos</t>
         </is>
       </c>
     </row>
@@ -1913,17 +1913,17 @@
         <v>45003</v>
       </c>
       <c r="B78" t="n">
-        <v>727</v>
+        <v>278</v>
       </c>
       <c r="C78" t="n">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Maquiagem</t>
         </is>
       </c>
     </row>
@@ -1932,17 +1932,17 @@
         <v>45004</v>
       </c>
       <c r="B79" t="n">
-        <v>141</v>
+        <v>610</v>
       </c>
       <c r="C79" t="n">
-        <v>463</v>
+        <v>337</v>
       </c>
       <c r="D79" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Águas</t>
         </is>
       </c>
     </row>
@@ -1951,17 +1951,17 @@
         <v>45005</v>
       </c>
       <c r="B80" t="n">
-        <v>926</v>
+        <v>559</v>
       </c>
       <c r="C80" t="n">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="D80" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Utensílios de Cozinha</t>
         </is>
       </c>
     </row>
@@ -1970,17 +1970,17 @@
         <v>45006</v>
       </c>
       <c r="B81" t="n">
-        <v>409</v>
+        <v>165</v>
       </c>
       <c r="C81" t="n">
-        <v>423</v>
+        <v>315</v>
       </c>
       <c r="D81" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Jardinagem</t>
         </is>
       </c>
     </row>
@@ -1989,17 +1989,17 @@
         <v>45007</v>
       </c>
       <c r="B82" t="n">
-        <v>472</v>
+        <v>594</v>
       </c>
       <c r="C82" t="n">
-        <v>217</v>
+        <v>129</v>
       </c>
       <c r="D82" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Esportes</t>
         </is>
       </c>
     </row>
@@ -2008,17 +2008,17 @@
         <v>45008</v>
       </c>
       <c r="B83" t="n">
-        <v>406</v>
+        <v>183</v>
       </c>
       <c r="C83" t="n">
-        <v>264</v>
+        <v>149</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Informática</t>
         </is>
       </c>
     </row>
@@ -2027,17 +2027,17 @@
         <v>45009</v>
       </c>
       <c r="B84" t="n">
-        <v>906</v>
+        <v>304</v>
       </c>
       <c r="C84" t="n">
-        <v>74</v>
+        <v>205</v>
       </c>
       <c r="D84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Jardinagem</t>
         </is>
       </c>
     </row>
@@ -2046,17 +2046,17 @@
         <v>45010</v>
       </c>
       <c r="B85" t="n">
-        <v>983</v>
+        <v>960</v>
       </c>
       <c r="C85" t="n">
-        <v>171</v>
+        <v>456</v>
       </c>
       <c r="D85" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Móveis</t>
         </is>
       </c>
     </row>
@@ -2065,17 +2065,17 @@
         <v>45011</v>
       </c>
       <c r="B86" t="n">
-        <v>204</v>
+        <v>673</v>
       </c>
       <c r="C86" t="n">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="D86" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Bebidas</t>
         </is>
       </c>
     </row>
@@ -2084,17 +2084,17 @@
         <v>45012</v>
       </c>
       <c r="B87" t="n">
-        <v>376</v>
+        <v>188</v>
       </c>
       <c r="C87" t="n">
-        <v>367</v>
+        <v>195</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
     </row>
@@ -2103,17 +2103,17 @@
         <v>45013</v>
       </c>
       <c r="B88" t="n">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C88" t="n">
-        <v>301</v>
+        <v>192</v>
       </c>
       <c r="D88" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Jogos</t>
+          <t>Chás</t>
         </is>
       </c>
     </row>
@@ -2122,17 +2122,17 @@
         <v>45014</v>
       </c>
       <c r="B89" t="n">
-        <v>924</v>
+        <v>145</v>
       </c>
       <c r="C89" t="n">
-        <v>107</v>
+        <v>395</v>
       </c>
       <c r="D89" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
     </row>
@@ -2141,17 +2141,17 @@
         <v>45015</v>
       </c>
       <c r="B90" t="n">
-        <v>999</v>
+        <v>475</v>
       </c>
       <c r="C90" t="n">
-        <v>367</v>
+        <v>256</v>
       </c>
       <c r="D90" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Jogos</t>
         </is>
       </c>
     </row>
@@ -2160,17 +2160,17 @@
         <v>45016</v>
       </c>
       <c r="B91" t="n">
-        <v>616</v>
+        <v>995</v>
       </c>
       <c r="C91" t="n">
-        <v>238</v>
+        <v>455</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>Celulares</t>
         </is>
       </c>
     </row>
@@ -2179,17 +2179,17 @@
         <v>45017</v>
       </c>
       <c r="B92" t="n">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="C92" t="n">
-        <v>262</v>
+        <v>352</v>
       </c>
       <c r="D92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Celulares</t>
         </is>
       </c>
     </row>
@@ -2198,17 +2198,17 @@
         <v>45018</v>
       </c>
       <c r="B93" t="n">
-        <v>919</v>
+        <v>336</v>
       </c>
       <c r="C93" t="n">
-        <v>95</v>
+        <v>408</v>
       </c>
       <c r="D93" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Roupas</t>
+          <t>Cereais</t>
         </is>
       </c>
     </row>
@@ -2217,17 +2217,17 @@
         <v>45019</v>
       </c>
       <c r="B94" t="n">
-        <v>255</v>
+        <v>601</v>
       </c>
       <c r="C94" t="n">
-        <v>151</v>
+        <v>409</v>
       </c>
       <c r="D94" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Jardinagem</t>
+          <t>Frutas</t>
         </is>
       </c>
     </row>
@@ -2236,17 +2236,17 @@
         <v>45020</v>
       </c>
       <c r="B95" t="n">
-        <v>570</v>
+        <v>618</v>
       </c>
       <c r="C95" t="n">
-        <v>475</v>
+        <v>302</v>
       </c>
       <c r="D95" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Decoração</t>
         </is>
       </c>
     </row>
@@ -2255,17 +2255,17 @@
         <v>45021</v>
       </c>
       <c r="B96" t="n">
-        <v>925</v>
+        <v>297</v>
       </c>
       <c r="C96" t="n">
-        <v>103</v>
+        <v>340</v>
       </c>
       <c r="D96" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Conservas</t>
         </is>
       </c>
     </row>
@@ -2274,17 +2274,17 @@
         <v>45022</v>
       </c>
       <c r="B97" t="n">
-        <v>947</v>
+        <v>619</v>
       </c>
       <c r="C97" t="n">
-        <v>464</v>
+        <v>64</v>
       </c>
       <c r="D97" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Móveis</t>
+          <t>Sorvetes</t>
         </is>
       </c>
     </row>
@@ -2293,17 +2293,17 @@
         <v>45023</v>
       </c>
       <c r="B98" t="n">
-        <v>726</v>
+        <v>858</v>
       </c>
       <c r="C98" t="n">
-        <v>491</v>
+        <v>389</v>
       </c>
       <c r="D98" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Chás</t>
         </is>
       </c>
     </row>
@@ -2312,17 +2312,17 @@
         <v>45024</v>
       </c>
       <c r="B99" t="n">
-        <v>164</v>
+        <v>754</v>
       </c>
       <c r="C99" t="n">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="D99" t="n">
         <v>8</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Esportes</t>
+          <t>Livros</t>
         </is>
       </c>
     </row>
@@ -2331,17 +2331,17 @@
         <v>45025</v>
       </c>
       <c r="B100" t="n">
-        <v>654</v>
+        <v>182</v>
       </c>
       <c r="C100" t="n">
-        <v>480</v>
+        <v>162</v>
       </c>
       <c r="D100" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Laticínios</t>
         </is>
       </c>
     </row>
@@ -2350,17 +2350,17 @@
         <v>45026</v>
       </c>
       <c r="B101" t="n">
-        <v>179</v>
+        <v>589</v>
       </c>
       <c r="C101" t="n">
-        <v>428</v>
+        <v>219</v>
       </c>
       <c r="D101" t="n">
         <v>8</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Café</t>
         </is>
       </c>
     </row>

</xml_diff>